<commit_message>
C: update the results, fix the mistake; re-run the panel analyses; done and prepared to public
</commit_message>
<xml_diff>
--- a/03_Results/04_03RE_SACMortalityLandCoverPanel.xlsx
+++ b/03_Results/04_03RE_SACMortalityLandCoverPanel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>X</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Total Impacts</t>
   </si>
   <si>
-    <t>Prevalence (confirmed/1000 cap)</t>
+    <t>Prevalence</t>
   </si>
   <si>
     <t/>
@@ -50,127 +50,130 @@
     <t>Time Lag of Mortality</t>
   </si>
   <si>
-    <t>0.012165***</t>
-  </si>
-  <si>
-    <t>(0.000282)</t>
-  </si>
-  <si>
-    <t>0.000875*</t>
-  </si>
-  <si>
-    <t>(0.000456)</t>
-  </si>
-  <si>
-    <t>-0.00185***</t>
-  </si>
-  <si>
-    <t>(0.000371)</t>
-  </si>
-  <si>
-    <t>-0.009601***</t>
-  </si>
-  <si>
-    <t>(0.000816)</t>
-  </si>
-  <si>
-    <t>0.007618***</t>
-  </si>
-  <si>
-    <t>(0.001216)</t>
-  </si>
-  <si>
-    <t>0.004715***</t>
-  </si>
-  <si>
-    <t>(0.000323)</t>
+    <t>0.012166***</t>
+  </si>
+  <si>
+    <t>(0.000291)</t>
+  </si>
+  <si>
+    <t>-0.000899*</t>
+  </si>
+  <si>
+    <t>(0.000477)</t>
+  </si>
+  <si>
+    <t>-0.005547***</t>
+  </si>
+  <si>
+    <t>(0.001112)</t>
+  </si>
+  <si>
+    <t>-0.028789***</t>
+  </si>
+  <si>
+    <t>(0.002458)</t>
+  </si>
+  <si>
+    <t>0.022852***</t>
+  </si>
+  <si>
+    <t>(0.003825)</t>
+  </si>
+  <si>
+    <t>0.004716***</t>
+  </si>
+  <si>
+    <t>(0.000319)</t>
   </si>
   <si>
     <t>-0.153623***</t>
   </si>
   <si>
-    <t>(0.007438)</t>
+    <t>(0.006957)</t>
   </si>
   <si>
     <t>-0.00549***</t>
   </si>
   <si>
+    <t>(0.000177)</t>
+  </si>
+  <si>
+    <t>0.000406*</t>
+  </si>
+  <si>
+    <t>(0.000216)</t>
+  </si>
+  <si>
+    <t>0.002503***</t>
+  </si>
+  <si>
+    <t>(0.000507)</t>
+  </si>
+  <si>
+    <t>0.012991***</t>
+  </si>
+  <si>
+    <t>(0.001142)</t>
+  </si>
+  <si>
+    <t>-0.010312***</t>
+  </si>
+  <si>
+    <t>(0.001748)</t>
+  </si>
+  <si>
+    <t>-0.002128***</t>
+  </si>
+  <si>
+    <t>(0.000152)</t>
+  </si>
+  <si>
+    <t>0.069323***</t>
+  </si>
+  <si>
+    <t>(0.003522)</t>
+  </si>
+  <si>
+    <t>0.006676***</t>
+  </si>
+  <si>
     <t>(0.00017)</t>
   </si>
   <si>
-    <t>-0.000395*</t>
-  </si>
-  <si>
-    <t>(0.000206)</t>
-  </si>
-  <si>
-    <t>0.000835***</t>
-  </si>
-  <si>
-    <t>(0.000168)</t>
-  </si>
-  <si>
-    <t>0.004333***</t>
-  </si>
-  <si>
-    <t>(0.000375)</t>
-  </si>
-  <si>
-    <t>-0.003438***</t>
-  </si>
-  <si>
-    <t>(0.000553)</t>
-  </si>
-  <si>
-    <t>-0.002128***</t>
-  </si>
-  <si>
-    <t>(0.000153)</t>
-  </si>
-  <si>
-    <t>0.069327***</t>
-  </si>
-  <si>
-    <t>(0.003619)</t>
-  </si>
-  <si>
-    <t>0.006675***</t>
-  </si>
-  <si>
-    <t>0.00048*</t>
-  </si>
-  <si>
-    <t>(0.00025)</t>
-  </si>
-  <si>
-    <t>-0.001015***</t>
-  </si>
-  <si>
-    <t>(0.000203)</t>
-  </si>
-  <si>
-    <t>-0.005268***</t>
-  </si>
-  <si>
-    <t>(0.000455)</t>
-  </si>
-  <si>
-    <t>0.00418***</t>
-  </si>
-  <si>
-    <t>(0.000668)</t>
-  </si>
-  <si>
-    <t>0.002587***</t>
-  </si>
-  <si>
-    <t>(0.000179)</t>
-  </si>
-  <si>
-    <t>-0.084296***</t>
-  </si>
-  <si>
-    <t>(0.004204)</t>
+    <t>-0.000493*</t>
+  </si>
+  <si>
+    <t>(0.000261)</t>
+  </si>
+  <si>
+    <t>-0.003044***</t>
+  </si>
+  <si>
+    <t>(0.000608)</t>
+  </si>
+  <si>
+    <t>-0.015798***</t>
+  </si>
+  <si>
+    <t>(0.001359)</t>
+  </si>
+  <si>
+    <t>0.01254***</t>
+  </si>
+  <si>
+    <t>(0.002094)</t>
+  </si>
+  <si>
+    <t>0.002588***</t>
+  </si>
+  <si>
+    <t>(0.000176)</t>
+  </si>
+  <si>
+    <t>-0.084301***</t>
+  </si>
+  <si>
+    <t>(0.003843)</t>
   </si>
 </sst>
 </file>
@@ -260,7 +263,7 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
@@ -274,7 +277,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
@@ -288,7 +291,7 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -302,7 +305,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
@@ -316,7 +319,7 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
@@ -330,7 +333,7 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -344,7 +347,7 @@
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10">
@@ -358,7 +361,7 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
@@ -372,7 +375,7 @@
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12">
@@ -386,7 +389,7 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -400,7 +403,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
@@ -414,7 +417,7 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
@@ -428,7 +431,7 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>